<commit_message>
Updated Afghanistan code with csv file at 10 km - for testing
</commit_message>
<xml_diff>
--- a/Afghanistan_ PyOnSSET/db/specs.xlsx
+++ b/Afghanistan_ PyOnSSET/db/specs.xlsx
@@ -567,7 +567,7 @@
         <v>7</v>
       </c>
       <c r="J2">
-        <v>0.69</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -594,7 +594,7 @@
         <v>0.3</v>
       </c>
       <c r="S2">
-        <v>0.381720623123198</v>
+        <v>0.7147033615400952</v>
       </c>
       <c r="T2">
         <v>60</v>

</xml_diff>

<commit_message>
Updaate of the specs file
</commit_message>
<xml_diff>
--- a/Afghanistan_ PyOnSSET/db/specs.xlsx
+++ b/Afghanistan_ PyOnSSET/db/specs.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alekor\Desktop\GithubClones\PyOnSSET\Afghanistan_ PyOnSSET\db\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -100,8 +105,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +169,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -210,7 +223,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -242,9 +255,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -276,6 +290,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -451,14 +466,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -538,7 +555,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
@@ -546,7 +563,7 @@
         <v>32527000</v>
       </c>
       <c r="C2">
-        <v>0.263</v>
+        <v>0.26300000000000001</v>
       </c>
       <c r="D2">
         <v>0.440916607491457</v>
@@ -555,10 +572,10 @@
         <v>44310000</v>
       </c>
       <c r="F2">
-        <v>0.358</v>
+        <v>0.35799999999999998</v>
       </c>
       <c r="G2">
-        <v>131.048772065437</v>
+        <v>131.04877206543699</v>
       </c>
       <c r="H2">
         <v>8.1</v>
@@ -567,13 +584,13 @@
         <v>7</v>
       </c>
       <c r="J2">
-        <v>0.6899999999999999</v>
+        <v>0.69</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.062</v>
+        <v>6.2E-2</v>
       </c>
       <c r="M2">
         <v>1722.01</v>
@@ -582,7 +599,7 @@
         <v>0.183</v>
       </c>
       <c r="O2">
-        <v>0.529580937</v>
+        <v>0.52958093699999997</v>
       </c>
       <c r="P2">
         <v>0.1</v>
@@ -594,19 +611,22 @@
         <v>0.3</v>
       </c>
       <c r="S2">
-        <v>0.7147033615400952</v>
+        <v>0.71470336154009517</v>
       </c>
       <c r="T2">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="U2">
         <v>5</v>
       </c>
+      <c r="V2">
+        <v>10</v>
+      </c>
       <c r="W2">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="X2">
-        <v>175</v>
+        <v>1500</v>
       </c>
       <c r="Y2">
         <v>10</v>

</xml_diff>